<commit_message>
Version 1.1: Actualizando Script para monitor, teclado y mouse
</commit_message>
<xml_diff>
--- a/Siati/inventarios_generados/Entrega_ADUANA-03.xlsx
+++ b/Siati/inventarios_generados/Entrega_ADUANA-03.xlsx
@@ -2733,7 +2733,7 @@
       <c r="Q9" s="231" t="n"/>
       <c r="R9" s="232" t="inlineStr">
         <is>
-          <t>11:07</t>
+          <t>12:12</t>
         </is>
       </c>
       <c r="S9" s="233" t="n"/>
@@ -3104,7 +3104,7 @@
       </c>
       <c r="B22" s="267" t="inlineStr">
         <is>
-          <t>Monitor</t>
+          <t>Teclado</t>
         </is>
       </c>
       <c r="C22" s="252" t="n"/>
@@ -3121,13 +3121,13 @@
       <c r="J22" s="253" t="n"/>
       <c r="K22" s="267" t="inlineStr">
         <is>
-          <t>(Standard monitor types)</t>
+          <t>Keyboard</t>
         </is>
       </c>
       <c r="L22" s="253" t="n"/>
       <c r="M22" s="267" t="inlineStr">
         <is>
-          <t>Generic Non-PnP Monitor</t>
+          <t>USB Input Device</t>
         </is>
       </c>
       <c r="N22" s="253" t="n"/>
@@ -3139,23 +3139,41 @@
       <c r="T22" s="208" t="n"/>
     </row>
     <row r="23" ht="99" customFormat="1" customHeight="1" s="204">
-      <c r="A23" s="266" t="n">
-        <v>3</v>
-      </c>
-      <c r="B23" s="267" t="n"/>
+      <c r="A23" s="266" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B23" s="267" t="inlineStr">
+        <is>
+          <t>Mouse</t>
+        </is>
+      </c>
       <c r="C23" s="252" t="n"/>
       <c r="D23" s="252" t="n"/>
       <c r="E23" s="252" t="n"/>
       <c r="F23" s="253" t="n"/>
       <c r="G23" s="267" t="n"/>
-      <c r="H23" s="267" t="n"/>
+      <c r="H23" s="267" t="inlineStr">
+        <is>
+          <t>En funcionamiento</t>
+        </is>
+      </c>
       <c r="I23" s="252" t="n"/>
       <c r="J23" s="253" t="n"/>
-      <c r="K23" s="267" t="n"/>
+      <c r="K23" s="267" t="inlineStr">
+        <is>
+          <t>Pointing</t>
+        </is>
+      </c>
       <c r="L23" s="253" t="n"/>
-      <c r="M23" s="267" t="n"/>
+      <c r="M23" s="267" t="inlineStr">
+        <is>
+          <t>USB Input Device</t>
+        </is>
+      </c>
       <c r="N23" s="253" t="n"/>
-      <c r="O23" s="268" t="n"/>
+      <c r="O23" s="268" t="inlineStr"/>
       <c r="P23" s="253" t="n"/>
       <c r="Q23" s="269" t="n"/>
       <c r="R23" s="252" t="n"/>

</xml_diff>